<commit_message>
enhance easyocr text testing results
</commit_message>
<xml_diff>
--- a/Results/result_comparison_summary.xlsx
+++ b/Results/result_comparison_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jerryliao/Jerry/Synechron/Projects/Recon_ai_sence/research/Tesseract_vs_EasyOCR/ocr_engines/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0FEB62-5D2C-5C41-B3EA-4E4AA4D14D3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CD2F70-AAD2-7B4C-8F37-951872799141}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15160" xr2:uid="{E8182C38-523F-DD45-8696-30A8DD0B12CA}"/>
+    <workbookView xWindow="1180" yWindow="1420" windowWidth="27240" windowHeight="15160" xr2:uid="{E8182C38-523F-DD45-8696-30A8DD0B12CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,14 +40,6 @@
 add , in the end</t>
   </si>
   <si>
-    <t>misinterpret b to o
-misinterpret h to n
-misinterpret f to t
-miss y in the end
-miss v
-miss entire word</t>
-  </si>
-  <si>
     <t>miss continuous 7
 miss continuous 2
 miss .</t>
@@ -67,6 +59,14 @@
   </si>
   <si>
     <t>Misinterpret Alphabets</t>
+  </si>
+  <si>
+    <t>misinterpret l to i
+misinterpret h to n
+misinterpret f to t
+misinterpret d to a
+miss y in the end
+miss v</t>
   </si>
 </sst>
 </file>
@@ -444,7 +444,7 @@
   <dimension ref="B1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -456,16 +456,16 @@
     <row r="2" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
       <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="85" x14ac:dyDescent="0.2">
@@ -479,7 +479,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>2</v>
@@ -493,13 +493,13 @@
         <v>1.9E-2</v>
       </c>
       <c r="D4" s="4">
-        <v>0.10199999999999999</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">

</xml_diff>